<commit_message>
Listado de artículos insight
</commit_message>
<xml_diff>
--- a/plantilla/DOCUMENTATION/LISTADO 100 ARTICULOS.xlsx
+++ b/plantilla/DOCUMENTATION/LISTADO 100 ARTICULOS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EderArmando\Documents\git\web-insight\plantilla\DOCUMENTATION\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="19875" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -893,12 +898,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1075,7 +1086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1182,6 +1193,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1193,6 +1213,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1241,7 +1264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1276,7 +1299,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1487,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1515,85 +1538,85 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="37">
+        <v>5</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="10"/>
@@ -2831,6 +2854,7 @@
     <hyperlink ref="B39" r:id="rId1" display="http://www.udca.edu.co/es/revista-cientifica/edicion-14-1-junio-2011/articulos-cientificos/1458-nuevo-metodo-ayuda-diagnostica-geometria-fractal-para-celulas-preneoplasicas-epitelio-escamoso-cervical.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="2833" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>